<commit_message>
escalation mails done need to set the time
</commit_message>
<xml_diff>
--- a/PR Master Template.xlsx
+++ b/PR Master Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Promptora\purchasekandhari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CABA86E-917A-482C-82E1-15A0F109A4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B94EF6-B9E7-4136-B6E6-683ADEE6BA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9B0CC429-ED49-4950-897D-A5C0295DABC0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>REQUISITIONNUMBER</t>
   </si>
@@ -122,13 +122,16 @@
   </si>
   <si>
     <t>LINESTATUS</t>
+  </si>
+  <si>
+    <t>VENDORACCOUNTNUMBER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +193,14 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -221,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -245,6 +256,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55DC462-D822-465F-B262-9C4FF45991DE}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="57" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,9 +692,10 @@
     <col min="21" max="21" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="39" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -752,20 +765,23 @@
       <c r="W1" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="X1" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="7" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -790,17 +806,17 @@
       <c r="V7" s="8"/>
       <c r="W7" s="8"/>
     </row>
-    <row r="8" spans="1:23" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="12"/>
       <c r="D8" s="4"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:23" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="10"/>
       <c r="E9" s="10"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="11" spans="1:23" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
     </row>
   </sheetData>

</xml_diff>